<commit_message>
Update readme and example for 1.1.0
</commit_message>
<xml_diff>
--- a/RDkit-QED/example_outputs/test_smiles_qed.xlsx
+++ b/RDkit-QED/example_outputs/test_smiles_qed.xlsx
@@ -1,26 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27231"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/85cb32c1384fb64c/Documents/GitHub/small-scripts/RDkit-QED/example_outputs/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="11_783E6D6494883EA4434B0304EFA0E5C8A9596FB4" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{174BBB47-6FCC-4486-B3A8-9B06414A2C22}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="88">
   <si>
     <t>PDB ID</t>
   </si>
@@ -49,9 +43,69 @@
     <t>ROMol</t>
   </si>
   <si>
+    <t>3DMol</t>
+  </si>
+  <si>
     <t>QED</t>
   </si>
   <si>
+    <t>MW</t>
+  </si>
+  <si>
+    <t>ALOGP</t>
+  </si>
+  <si>
+    <t>HBA</t>
+  </si>
+  <si>
+    <t>HBD</t>
+  </si>
+  <si>
+    <t>PSA</t>
+  </si>
+  <si>
+    <t>ROTB</t>
+  </si>
+  <si>
+    <t>AROM</t>
+  </si>
+  <si>
+    <t>ALERTS</t>
+  </si>
+  <si>
+    <t>Num Ring</t>
+  </si>
+  <si>
+    <t>Num Ar Ring</t>
+  </si>
+  <si>
+    <t>Num ArHetcy</t>
+  </si>
+  <si>
+    <t>Num Hetcy</t>
+  </si>
+  <si>
+    <t>Num Hetatm</t>
+  </si>
+  <si>
+    <t>Num Spiro</t>
+  </si>
+  <si>
+    <t>Frac Sp3</t>
+  </si>
+  <si>
+    <t>MR</t>
+  </si>
+  <si>
+    <t>NPR1</t>
+  </si>
+  <si>
+    <t>NPR2</t>
+  </si>
+  <si>
+    <t>Geometry</t>
+  </si>
+  <si>
     <t>1P9X</t>
   </si>
   <si>
@@ -70,6 +124,9 @@
     <t>CCC1C2(C(C(C(=O)C(CC(C(C(C(=O)C(C(=O)O1)C)C)OC3C(C(CC(O3)C)N(C)C)O)(C)OC)C)C)N(C(=O)O2)CCCCn4cc(nc4)c5cccnc5)C</t>
   </si>
   <si>
+    <t>Rod-like</t>
+  </si>
+  <si>
     <t>2O44</t>
   </si>
   <si>
@@ -110,6 +167,9 @@
   </si>
   <si>
     <t>c1c2c(nc(n1)N)n(cn2)C3C(C(C(O3)CO)O)O</t>
+  </si>
+  <si>
+    <t>Balanced</t>
   </si>
   <si>
     <t>7XD7</t>
@@ -223,8 +283,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -261,14 +321,6 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -289,13 +341,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1" descr="f">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
+        <xdr:cNvPr id="2" name="Picture 1" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -320,6 +366,44 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>1428750</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>1428750</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2" descr="f"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6591300" y="190500"/>
+          <a:ext cx="1428750" cy="1428750"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
       <xdr:col>8</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>2</xdr:row>
@@ -333,19 +417,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Picture 2" descr="f">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
+        <xdr:cNvPr id="4" name="Picture 3" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -353,6 +431,44 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="4876800" y="2095500"/>
+          <a:ext cx="1428750" cy="1428750"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>1428750</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>1428750</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Picture 4" descr="f"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6591300" y="2095500"/>
           <a:ext cx="1428750" cy="1428750"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -377,19 +493,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="4" name="Picture 3" descr="f">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000004000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
+        <xdr:cNvPr id="6" name="Picture 5" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -397,6 +507,44 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="4876800" y="4000500"/>
+          <a:ext cx="1428750" cy="1428750"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>1428750</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>1428750</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="7" name="Picture 6" descr="f"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6591300" y="4000500"/>
           <a:ext cx="1428750" cy="1428750"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -421,19 +569,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="5" name="Picture 4" descr="f">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000005000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
+        <xdr:cNvPr id="8" name="Picture 7" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -441,6 +583,44 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="4876800" y="5905500"/>
+          <a:ext cx="1428750" cy="1428750"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>1428750</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>1428750</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="9" name="Picture 8" descr="f"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6591300" y="5905500"/>
           <a:ext cx="1428750" cy="1428750"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -465,19 +645,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="6" name="Picture 5" descr="f">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000006000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
+        <xdr:cNvPr id="10" name="Picture 9" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -485,6 +659,44 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="4876800" y="7810500"/>
+          <a:ext cx="1428750" cy="1428750"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>1428750</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>1428750</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="11" name="Picture 10" descr="f"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId9"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6591300" y="7810500"/>
           <a:ext cx="1428750" cy="1428750"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -509,19 +721,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="7" name="Picture 6" descr="f">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000007000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
+        <xdr:cNvPr id="12" name="Picture 11" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId10"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -529,6 +735,44 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="4876800" y="9715500"/>
+          <a:ext cx="1428750" cy="1428750"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>1428750</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>1428750</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="13" name="Picture 12" descr="f"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId11"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6591300" y="9715500"/>
           <a:ext cx="1428750" cy="1428750"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -553,19 +797,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="8" name="Picture 7" descr="f">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000008000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
+        <xdr:cNvPr id="14" name="Picture 13" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId12"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -573,6 +811,44 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="4876800" y="11620500"/>
+          <a:ext cx="1428750" cy="1428750"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>1428750</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>1428750</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="15" name="Picture 14" descr="f"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId13"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6591300" y="11620500"/>
           <a:ext cx="1428750" cy="1428750"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -597,19 +873,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="9" name="Picture 8" descr="f">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000009000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
+        <xdr:cNvPr id="16" name="Picture 15" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId10"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -617,6 +887,44 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="4876800" y="13525500"/>
+          <a:ext cx="1428750" cy="1428750"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>1428750</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>1428750</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="17" name="Picture 16" descr="f"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId14"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6591300" y="13525500"/>
           <a:ext cx="1428750" cy="1428750"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -641,19 +949,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="10" name="Picture 9" descr="f">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000A000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
+        <xdr:cNvPr id="18" name="Picture 17" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId10"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -661,6 +963,44 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="4876800" y="15430500"/>
+          <a:ext cx="1428750" cy="1428750"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>1428750</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>1428750</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="19" name="Picture 18" descr="f"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId15"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6591300" y="15430500"/>
           <a:ext cx="1428750" cy="1428750"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -685,19 +1025,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="11" name="Picture 10" descr="f">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000B000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
+        <xdr:cNvPr id="20" name="Picture 19" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -705,6 +1039,44 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="4876800" y="17335500"/>
+          <a:ext cx="1428750" cy="1428750"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>1428750</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>1428750</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="21" name="Picture 20" descr="f"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId16"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6591300" y="17335500"/>
           <a:ext cx="1428750" cy="1428750"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -729,19 +1101,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="12" name="Picture 11" descr="f">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000C000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
+        <xdr:cNvPr id="22" name="Picture 21" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId12"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -749,6 +1115,44 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="4876800" y="19240500"/>
+          <a:ext cx="1428750" cy="1428750"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>1428750</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>1428750</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="23" name="Picture 22" descr="f"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId17"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6591300" y="19240500"/>
           <a:ext cx="1428750" cy="1428750"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -773,19 +1177,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="13" name="Picture 12" descr="f">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000D000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
+        <xdr:cNvPr id="24" name="Picture 23" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId10"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -793,6 +1191,44 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="4876800" y="21145500"/>
+          <a:ext cx="1428750" cy="1428750"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>1428750</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>1428750</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="25" name="Picture 24" descr="f"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId18"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6591300" y="21145500"/>
           <a:ext cx="1428750" cy="1428750"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -817,19 +1253,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="14" name="Picture 13" descr="f">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000E000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
+        <xdr:cNvPr id="26" name="Picture 25" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId12"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -837,6 +1267,44 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="4876800" y="23050500"/>
+          <a:ext cx="1428750" cy="1428750"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>1428750</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>1428750</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="27" name="Picture 26" descr="f"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId19"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6591300" y="23050500"/>
           <a:ext cx="1428750" cy="1428750"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -861,19 +1329,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="15" name="Picture 14" descr="f">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000F000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
+        <xdr:cNvPr id="28" name="Picture 27" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId10"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -881,6 +1343,44 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="4876800" y="24955500"/>
+          <a:ext cx="1428750" cy="1428750"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>1428750</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>1428750</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="29" name="Picture 28" descr="f"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId20"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6591300" y="24955500"/>
           <a:ext cx="1428750" cy="1428750"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -905,19 +1405,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="16" name="Picture 15" descr="f">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000010000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
+        <xdr:cNvPr id="30" name="Picture 29" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId10"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -925,6 +1419,44 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="4876800" y="26860500"/>
+          <a:ext cx="1428750" cy="1428750"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>1428750</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>1428750</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="31" name="Picture 30" descr="f"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId21"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6591300" y="26860500"/>
           <a:ext cx="1428750" cy="1428750"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -949,19 +1481,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="17" name="Picture 16" descr="f">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000011000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
+        <xdr:cNvPr id="32" name="Picture 31" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId10"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -969,6 +1495,44 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="4876800" y="28765500"/>
+          <a:ext cx="1428750" cy="1428750"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>1428750</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>1428750</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="33" name="Picture 32" descr="f"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId22"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6591300" y="28765500"/>
           <a:ext cx="1428750" cy="1428750"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -993,19 +1557,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="18" name="Picture 17" descr="f">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000012000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
+        <xdr:cNvPr id="34" name="Picture 33" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId12"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -1013,6 +1571,44 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="4876800" y="30670500"/>
+          <a:ext cx="1428750" cy="1428750"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>1428750</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>1428750</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="35" name="Picture 34" descr="f"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId23"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6591300" y="30670500"/>
           <a:ext cx="1428750" cy="1428750"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1037,19 +1633,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="19" name="Picture 18" descr="f">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000013000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
+        <xdr:cNvPr id="36" name="Picture 35" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId12"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -1057,6 +1647,44 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="4876800" y="32575500"/>
+          <a:ext cx="1428750" cy="1428750"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>1428750</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>1428750</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="37" name="Picture 36" descr="f"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId24"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6591300" y="32575500"/>
           <a:ext cx="1428750" cy="1428750"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1081,19 +1709,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="20" name="Picture 19" descr="f">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000014000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
+        <xdr:cNvPr id="38" name="Picture 37" descr="f"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId10"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -1110,13 +1732,51 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>1428750</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>1428750</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="39" name="Picture 38" descr="f"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId25"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6591300" y="34480500"/>
+          <a:ext cx="1428750" cy="1428750"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2007 - 2010">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1154,7 +1814,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2007 - 2010">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -1188,7 +1848,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -1223,10 +1882,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2007 - 2010">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1399,20 +2057,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J20"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:AD20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="8" max="8" width="110" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="25.6640625" customWidth="1"/>
+    <col min="9" max="10" width="25.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:30">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1443,161 +2098,506 @@
       <c r="J1" t="s">
         <v>9</v>
       </c>
+      <c r="K1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>16</v>
+      </c>
+      <c r="R1" t="s">
+        <v>17</v>
+      </c>
+      <c r="S1" t="s">
+        <v>18</v>
+      </c>
+      <c r="T1" t="s">
+        <v>19</v>
+      </c>
+      <c r="U1" t="s">
+        <v>20</v>
+      </c>
+      <c r="V1" t="s">
+        <v>21</v>
+      </c>
+      <c r="W1" t="s">
+        <v>22</v>
+      </c>
+      <c r="X1" t="s">
+        <v>23</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>24</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>25</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>26</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>27</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>28</v>
+      </c>
+      <c r="AD1" t="s">
+        <v>29</v>
+      </c>
     </row>
-    <row r="2" spans="1:10" ht="150" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:30" ht="150" customHeight="1">
       <c r="A2" t="s">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="B2" t="s">
-        <v>11</v>
+        <v>31</v>
       </c>
       <c r="C2" t="s">
-        <v>12</v>
+        <v>32</v>
       </c>
       <c r="D2">
         <v>2880</v>
       </c>
       <c r="E2">
-        <v>933.40499999999997</v>
+        <v>933.405</v>
       </c>
       <c r="F2" t="s">
+        <v>33</v>
+      </c>
+      <c r="G2" t="s">
+        <v>34</v>
+      </c>
+      <c r="H2" t="s">
+        <v>35</v>
+      </c>
+      <c r="K2">
+        <v>0.1842834348292615</v>
+      </c>
+      <c r="L2">
+        <v>812.0179999999997</v>
+      </c>
+      <c r="M2">
+        <v>4.929200000000005</v>
+      </c>
+      <c r="N2">
         <v>13</v>
       </c>
-      <c r="G2" t="s">
-        <v>14</v>
-      </c>
-      <c r="H2" t="s">
+      <c r="O2">
+        <v>1</v>
+      </c>
+      <c r="P2">
+        <v>171.85</v>
+      </c>
+      <c r="Q2">
+        <v>11</v>
+      </c>
+      <c r="R2">
+        <v>2</v>
+      </c>
+      <c r="S2">
+        <v>3</v>
+      </c>
+      <c r="T2">
+        <v>5</v>
+      </c>
+      <c r="U2">
+        <v>2</v>
+      </c>
+      <c r="V2">
+        <v>2</v>
+      </c>
+      <c r="W2">
+        <v>5</v>
+      </c>
+      <c r="X2">
         <v>15</v>
       </c>
-      <c r="J2">
-        <v>0.18428343482926149</v>
+      <c r="Y2">
+        <v>0</v>
+      </c>
+      <c r="Z2">
+        <v>0.7209302325581395</v>
+      </c>
+      <c r="AA2">
+        <v>214.2507999999992</v>
+      </c>
+      <c r="AB2">
+        <v>0.3200665826495543</v>
+      </c>
+      <c r="AC2">
+        <v>0.9183353876285404</v>
+      </c>
+      <c r="AD2" t="s">
+        <v>36</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="150" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:30" ht="150" customHeight="1">
       <c r="A3" t="s">
-        <v>16</v>
+        <v>37</v>
       </c>
       <c r="B3" t="s">
-        <v>17</v>
+        <v>38</v>
       </c>
       <c r="C3" t="s">
-        <v>12</v>
+        <v>32</v>
       </c>
       <c r="D3">
         <v>2880</v>
       </c>
       <c r="E3">
-        <v>933.40499999999997</v>
+        <v>933.405</v>
       </c>
       <c r="F3" t="s">
-        <v>18</v>
+        <v>39</v>
       </c>
       <c r="G3" t="s">
-        <v>19</v>
+        <v>40</v>
       </c>
       <c r="H3" t="s">
-        <v>20</v>
-      </c>
-      <c r="J3">
+        <v>41</v>
+      </c>
+      <c r="K3">
         <v>0.1469366180673812</v>
       </c>
+      <c r="L3">
+        <v>828.0060000000001</v>
+      </c>
+      <c r="M3">
+        <v>3.013400000000005</v>
+      </c>
+      <c r="N3">
+        <v>16</v>
+      </c>
+      <c r="O3">
+        <v>3</v>
+      </c>
+      <c r="P3">
+        <v>206.05</v>
+      </c>
+      <c r="Q3">
+        <v>12</v>
+      </c>
+      <c r="R3">
+        <v>0</v>
+      </c>
+      <c r="S3">
+        <v>3</v>
+      </c>
+      <c r="T3">
+        <v>3</v>
+      </c>
+      <c r="U3">
+        <v>0</v>
+      </c>
+      <c r="V3">
+        <v>0</v>
+      </c>
+      <c r="W3">
+        <v>3</v>
+      </c>
+      <c r="X3">
+        <v>16</v>
+      </c>
+      <c r="Y3">
+        <v>0</v>
+      </c>
+      <c r="Z3">
+        <v>0.8095238095238095</v>
+      </c>
+      <c r="AA3">
+        <v>209.8513999999991</v>
+      </c>
+      <c r="AB3">
+        <v>0.2791562186178549</v>
+      </c>
+      <c r="AC3">
+        <v>0.9765657748562725</v>
+      </c>
+      <c r="AD3" t="s">
+        <v>36</v>
+      </c>
     </row>
-    <row r="4" spans="1:10" ht="150" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:30" ht="150" customHeight="1">
       <c r="A4" t="s">
-        <v>21</v>
+        <v>42</v>
       </c>
       <c r="B4" t="s">
-        <v>22</v>
+        <v>43</v>
       </c>
       <c r="C4" t="s">
-        <v>23</v>
+        <v>44</v>
       </c>
       <c r="D4">
         <v>418</v>
       </c>
       <c r="E4">
-        <v>134.81100000000001</v>
+        <v>134.811</v>
       </c>
       <c r="F4" t="s">
-        <v>24</v>
+        <v>45</v>
       </c>
       <c r="G4" t="s">
-        <v>25</v>
+        <v>46</v>
       </c>
       <c r="H4" t="s">
-        <v>26</v>
-      </c>
-      <c r="J4">
-        <v>0.42954372454005812</v>
+        <v>47</v>
+      </c>
+      <c r="K4">
+        <v>0.4295437245400581</v>
+      </c>
+      <c r="L4">
+        <v>145.25</v>
+      </c>
+      <c r="M4">
+        <v>-0.3362999999999984</v>
+      </c>
+      <c r="N4">
+        <v>3</v>
+      </c>
+      <c r="O4">
+        <v>3</v>
+      </c>
+      <c r="P4">
+        <v>64.06999999999999</v>
+      </c>
+      <c r="Q4">
+        <v>7</v>
+      </c>
+      <c r="R4">
+        <v>0</v>
+      </c>
+      <c r="S4">
+        <v>1</v>
+      </c>
+      <c r="T4">
+        <v>0</v>
+      </c>
+      <c r="U4">
+        <v>0</v>
+      </c>
+      <c r="V4">
+        <v>0</v>
+      </c>
+      <c r="W4">
+        <v>0</v>
+      </c>
+      <c r="X4">
+        <v>3</v>
+      </c>
+      <c r="Y4">
+        <v>0</v>
+      </c>
+      <c r="Z4">
+        <v>1</v>
+      </c>
+      <c r="AA4">
+        <v>44.8295</v>
+      </c>
+      <c r="AB4">
+        <v>0.05727630689486384</v>
+      </c>
+      <c r="AC4">
+        <v>0.9776372649151569</v>
+      </c>
+      <c r="AD4" t="s">
+        <v>36</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="150" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:30" ht="150" customHeight="1">
       <c r="A5" t="s">
-        <v>21</v>
+        <v>42</v>
       </c>
       <c r="B5" t="s">
-        <v>22</v>
+        <v>43</v>
       </c>
       <c r="C5" t="s">
-        <v>23</v>
+        <v>44</v>
       </c>
       <c r="D5">
         <v>418</v>
       </c>
       <c r="E5">
-        <v>134.81100000000001</v>
+        <v>134.811</v>
       </c>
       <c r="F5" t="s">
-        <v>27</v>
+        <v>48</v>
       </c>
       <c r="G5" t="s">
-        <v>28</v>
+        <v>49</v>
       </c>
       <c r="H5" t="s">
-        <v>29</v>
-      </c>
-      <c r="J5">
-        <v>0.49051986767922318</v>
+        <v>50</v>
+      </c>
+      <c r="K5">
+        <v>0.4905198676792232</v>
+      </c>
+      <c r="L5">
+        <v>267.245</v>
+      </c>
+      <c r="M5">
+        <v>-1.980000000000001</v>
+      </c>
+      <c r="N5">
+        <v>8</v>
+      </c>
+      <c r="O5">
+        <v>4</v>
+      </c>
+      <c r="P5">
+        <v>139.54</v>
+      </c>
+      <c r="Q5">
+        <v>2</v>
+      </c>
+      <c r="R5">
+        <v>2</v>
+      </c>
+      <c r="S5">
+        <v>0</v>
+      </c>
+      <c r="T5">
+        <v>3</v>
+      </c>
+      <c r="U5">
+        <v>2</v>
+      </c>
+      <c r="V5">
+        <v>2</v>
+      </c>
+      <c r="W5">
+        <v>3</v>
+      </c>
+      <c r="X5">
+        <v>9</v>
+      </c>
+      <c r="Y5">
+        <v>0</v>
+      </c>
+      <c r="Z5">
+        <v>0.5</v>
+      </c>
+      <c r="AA5">
+        <v>62.74480000000002</v>
+      </c>
+      <c r="AB5">
+        <v>0.3226667734247431</v>
+      </c>
+      <c r="AC5">
+        <v>0.8002816697850615</v>
+      </c>
+      <c r="AD5" t="s">
+        <v>51</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="150" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:30" ht="150" customHeight="1">
       <c r="A6" t="s">
-        <v>30</v>
+        <v>52</v>
       </c>
       <c r="B6" t="s">
-        <v>31</v>
+        <v>53</v>
       </c>
       <c r="C6" t="s">
-        <v>32</v>
+        <v>54</v>
       </c>
       <c r="D6">
         <v>405</v>
       </c>
       <c r="E6">
-        <v>130.73500000000001</v>
+        <v>130.735</v>
       </c>
       <c r="F6" t="s">
-        <v>24</v>
+        <v>45</v>
       </c>
       <c r="G6" t="s">
-        <v>25</v>
+        <v>46</v>
       </c>
       <c r="H6" t="s">
-        <v>26</v>
-      </c>
-      <c r="J6">
-        <v>0.42954372454005812</v>
+        <v>47</v>
+      </c>
+      <c r="K6">
+        <v>0.4295437245400581</v>
+      </c>
+      <c r="L6">
+        <v>145.25</v>
+      </c>
+      <c r="M6">
+        <v>-0.3362999999999984</v>
+      </c>
+      <c r="N6">
+        <v>3</v>
+      </c>
+      <c r="O6">
+        <v>3</v>
+      </c>
+      <c r="P6">
+        <v>64.06999999999999</v>
+      </c>
+      <c r="Q6">
+        <v>7</v>
+      </c>
+      <c r="R6">
+        <v>0</v>
+      </c>
+      <c r="S6">
+        <v>1</v>
+      </c>
+      <c r="T6">
+        <v>0</v>
+      </c>
+      <c r="U6">
+        <v>0</v>
+      </c>
+      <c r="V6">
+        <v>0</v>
+      </c>
+      <c r="W6">
+        <v>0</v>
+      </c>
+      <c r="X6">
+        <v>3</v>
+      </c>
+      <c r="Y6">
+        <v>0</v>
+      </c>
+      <c r="Z6">
+        <v>1</v>
+      </c>
+      <c r="AA6">
+        <v>44.8295</v>
+      </c>
+      <c r="AB6">
+        <v>0.05629636783265283</v>
+      </c>
+      <c r="AC6">
+        <v>0.9712753743770466</v>
+      </c>
+      <c r="AD6" t="s">
+        <v>36</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="150" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:30" ht="150" customHeight="1">
       <c r="A7" t="s">
-        <v>33</v>
+        <v>55</v>
       </c>
       <c r="B7" t="s">
-        <v>34</v>
+        <v>56</v>
       </c>
       <c r="C7" t="s">
-        <v>35</v>
+        <v>57</v>
       </c>
       <c r="D7">
         <v>398</v>
@@ -1606,27 +2606,84 @@
         <v>129.28</v>
       </c>
       <c r="F7" t="s">
+        <v>58</v>
+      </c>
+      <c r="G7" t="s">
+        <v>59</v>
+      </c>
+      <c r="H7" t="s">
+        <v>60</v>
+      </c>
+      <c r="K7">
+        <v>0.5664580841045198</v>
+      </c>
+      <c r="L7">
+        <v>238.309</v>
+      </c>
+      <c r="M7">
+        <v>-1.515899999999997</v>
+      </c>
+      <c r="N7">
+        <v>6</v>
+      </c>
+      <c r="O7">
+        <v>2</v>
+      </c>
+      <c r="P7">
+        <v>81.08</v>
+      </c>
+      <c r="Q7">
+        <v>5</v>
+      </c>
+      <c r="R7">
+        <v>0</v>
+      </c>
+      <c r="S7">
+        <v>1</v>
+      </c>
+      <c r="T7">
+        <v>1</v>
+      </c>
+      <c r="U7">
+        <v>0</v>
+      </c>
+      <c r="V7">
+        <v>0</v>
+      </c>
+      <c r="W7">
+        <v>1</v>
+      </c>
+      <c r="X7">
+        <v>7</v>
+      </c>
+      <c r="Y7">
+        <v>0</v>
+      </c>
+      <c r="Z7">
+        <v>1</v>
+      </c>
+      <c r="AA7">
+        <v>56.38140000000003</v>
+      </c>
+      <c r="AB7">
+        <v>0.1480550974144793</v>
+      </c>
+      <c r="AC7">
+        <v>0.9658446502942545</v>
+      </c>
+      <c r="AD7" t="s">
         <v>36</v>
       </c>
-      <c r="G7" t="s">
-        <v>37</v>
-      </c>
-      <c r="H7" t="s">
-        <v>38</v>
-      </c>
-      <c r="J7">
-        <v>0.56645808410451981</v>
-      </c>
     </row>
-    <row r="8" spans="1:10" ht="150" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:30" ht="150" customHeight="1">
       <c r="A8" t="s">
-        <v>39</v>
+        <v>61</v>
       </c>
       <c r="B8" t="s">
-        <v>40</v>
+        <v>62</v>
       </c>
       <c r="C8" t="s">
-        <v>41</v>
+        <v>63</v>
       </c>
       <c r="D8">
         <v>398</v>
@@ -1635,27 +2692,84 @@
         <v>129.24</v>
       </c>
       <c r="F8" t="s">
-        <v>42</v>
+        <v>64</v>
       </c>
       <c r="G8" t="s">
-        <v>43</v>
+        <v>65</v>
       </c>
       <c r="H8" t="s">
-        <v>44</v>
-      </c>
-      <c r="J8">
+        <v>66</v>
+      </c>
+      <c r="K8">
         <v>0.3452806057714905</v>
       </c>
+      <c r="L8">
+        <v>202.346</v>
+      </c>
+      <c r="M8">
+        <v>-0.3565999999999975</v>
+      </c>
+      <c r="N8">
+        <v>4</v>
+      </c>
+      <c r="O8">
+        <v>4</v>
+      </c>
+      <c r="P8">
+        <v>76.09999999999999</v>
+      </c>
+      <c r="Q8">
+        <v>11</v>
+      </c>
+      <c r="R8">
+        <v>0</v>
+      </c>
+      <c r="S8">
+        <v>1</v>
+      </c>
+      <c r="T8">
+        <v>0</v>
+      </c>
+      <c r="U8">
+        <v>0</v>
+      </c>
+      <c r="V8">
+        <v>0</v>
+      </c>
+      <c r="W8">
+        <v>0</v>
+      </c>
+      <c r="X8">
+        <v>4</v>
+      </c>
+      <c r="Y8">
+        <v>0</v>
+      </c>
+      <c r="Z8">
+        <v>1</v>
+      </c>
+      <c r="AA8">
+        <v>62.31620000000004</v>
+      </c>
+      <c r="AB8">
+        <v>0.1611115032444971</v>
+      </c>
+      <c r="AC8">
+        <v>0.9035963444505466</v>
+      </c>
+      <c r="AD8" t="s">
+        <v>36</v>
+      </c>
     </row>
-    <row r="9" spans="1:10" ht="150" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:30" ht="150" customHeight="1">
       <c r="A9" t="s">
-        <v>39</v>
+        <v>61</v>
       </c>
       <c r="B9" t="s">
-        <v>40</v>
+        <v>62</v>
       </c>
       <c r="C9" t="s">
-        <v>41</v>
+        <v>63</v>
       </c>
       <c r="D9">
         <v>398</v>
@@ -1664,143 +2778,428 @@
         <v>129.24</v>
       </c>
       <c r="F9" t="s">
+        <v>58</v>
+      </c>
+      <c r="G9" t="s">
+        <v>59</v>
+      </c>
+      <c r="H9" t="s">
+        <v>60</v>
+      </c>
+      <c r="K9">
+        <v>0.5664580841045198</v>
+      </c>
+      <c r="L9">
+        <v>238.309</v>
+      </c>
+      <c r="M9">
+        <v>-1.515899999999997</v>
+      </c>
+      <c r="N9">
+        <v>6</v>
+      </c>
+      <c r="O9">
+        <v>2</v>
+      </c>
+      <c r="P9">
+        <v>81.08</v>
+      </c>
+      <c r="Q9">
+        <v>5</v>
+      </c>
+      <c r="R9">
+        <v>0</v>
+      </c>
+      <c r="S9">
+        <v>1</v>
+      </c>
+      <c r="T9">
+        <v>1</v>
+      </c>
+      <c r="U9">
+        <v>0</v>
+      </c>
+      <c r="V9">
+        <v>0</v>
+      </c>
+      <c r="W9">
+        <v>1</v>
+      </c>
+      <c r="X9">
+        <v>7</v>
+      </c>
+      <c r="Y9">
+        <v>0</v>
+      </c>
+      <c r="Z9">
+        <v>1</v>
+      </c>
+      <c r="AA9">
+        <v>56.38140000000003</v>
+      </c>
+      <c r="AB9">
+        <v>0.2577886776515536</v>
+      </c>
+      <c r="AC9">
+        <v>0.9215850671339433</v>
+      </c>
+      <c r="AD9" t="s">
         <v>36</v>
       </c>
-      <c r="G9" t="s">
-        <v>37</v>
-      </c>
-      <c r="H9" t="s">
-        <v>38</v>
-      </c>
-      <c r="J9">
-        <v>0.56645808410451981</v>
-      </c>
     </row>
-    <row r="10" spans="1:10" ht="150" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:30" ht="150" customHeight="1">
       <c r="A10" t="s">
-        <v>45</v>
+        <v>67</v>
       </c>
       <c r="B10" t="s">
-        <v>46</v>
+        <v>68</v>
       </c>
       <c r="C10" t="s">
-        <v>47</v>
+        <v>69</v>
       </c>
       <c r="D10">
         <v>398</v>
       </c>
       <c r="E10">
-        <v>129.22499999999999</v>
+        <v>129.225</v>
       </c>
       <c r="F10" t="s">
+        <v>58</v>
+      </c>
+      <c r="G10" t="s">
+        <v>59</v>
+      </c>
+      <c r="H10" t="s">
+        <v>60</v>
+      </c>
+      <c r="K10">
+        <v>0.5664580841045198</v>
+      </c>
+      <c r="L10">
+        <v>238.309</v>
+      </c>
+      <c r="M10">
+        <v>-1.515899999999997</v>
+      </c>
+      <c r="N10">
+        <v>6</v>
+      </c>
+      <c r="O10">
+        <v>2</v>
+      </c>
+      <c r="P10">
+        <v>81.08</v>
+      </c>
+      <c r="Q10">
+        <v>5</v>
+      </c>
+      <c r="R10">
+        <v>0</v>
+      </c>
+      <c r="S10">
+        <v>1</v>
+      </c>
+      <c r="T10">
+        <v>1</v>
+      </c>
+      <c r="U10">
+        <v>0</v>
+      </c>
+      <c r="V10">
+        <v>0</v>
+      </c>
+      <c r="W10">
+        <v>1</v>
+      </c>
+      <c r="X10">
+        <v>7</v>
+      </c>
+      <c r="Y10">
+        <v>0</v>
+      </c>
+      <c r="Z10">
+        <v>1</v>
+      </c>
+      <c r="AA10">
+        <v>56.38140000000003</v>
+      </c>
+      <c r="AB10">
+        <v>0.1188504204109976</v>
+      </c>
+      <c r="AC10">
+        <v>0.960542170321001</v>
+      </c>
+      <c r="AD10" t="s">
         <v>36</v>
       </c>
-      <c r="G10" t="s">
-        <v>37</v>
-      </c>
-      <c r="H10" t="s">
-        <v>38</v>
-      </c>
-      <c r="J10">
-        <v>0.56645808410451981</v>
-      </c>
     </row>
-    <row r="11" spans="1:10" ht="150" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:30" ht="150" customHeight="1">
       <c r="A11" t="s">
-        <v>48</v>
+        <v>70</v>
       </c>
       <c r="B11" t="s">
-        <v>49</v>
+        <v>71</v>
       </c>
       <c r="C11" t="s">
-        <v>50</v>
+        <v>72</v>
       </c>
       <c r="D11">
         <v>400</v>
       </c>
       <c r="E11">
-        <v>129.22200000000001</v>
+        <v>129.222</v>
       </c>
       <c r="F11" t="s">
-        <v>24</v>
+        <v>45</v>
       </c>
       <c r="G11" t="s">
-        <v>25</v>
+        <v>46</v>
       </c>
       <c r="H11" t="s">
-        <v>26</v>
-      </c>
-      <c r="J11">
-        <v>0.42954372454005812</v>
+        <v>47</v>
+      </c>
+      <c r="K11">
+        <v>0.4295437245400581</v>
+      </c>
+      <c r="L11">
+        <v>145.25</v>
+      </c>
+      <c r="M11">
+        <v>-0.3362999999999984</v>
+      </c>
+      <c r="N11">
+        <v>3</v>
+      </c>
+      <c r="O11">
+        <v>3</v>
+      </c>
+      <c r="P11">
+        <v>64.06999999999999</v>
+      </c>
+      <c r="Q11">
+        <v>7</v>
+      </c>
+      <c r="R11">
+        <v>0</v>
+      </c>
+      <c r="S11">
+        <v>1</v>
+      </c>
+      <c r="T11">
+        <v>0</v>
+      </c>
+      <c r="U11">
+        <v>0</v>
+      </c>
+      <c r="V11">
+        <v>0</v>
+      </c>
+      <c r="W11">
+        <v>0</v>
+      </c>
+      <c r="X11">
+        <v>3</v>
+      </c>
+      <c r="Y11">
+        <v>0</v>
+      </c>
+      <c r="Z11">
+        <v>1</v>
+      </c>
+      <c r="AA11">
+        <v>44.8295</v>
+      </c>
+      <c r="AB11">
+        <v>0.1788465291257333</v>
+      </c>
+      <c r="AC11">
+        <v>0.8912868155753061</v>
+      </c>
+      <c r="AD11" t="s">
+        <v>36</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="150" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:30" ht="150" customHeight="1">
       <c r="A12" t="s">
-        <v>51</v>
+        <v>73</v>
       </c>
       <c r="B12" t="s">
-        <v>52</v>
+        <v>74</v>
       </c>
       <c r="C12" t="s">
-        <v>53</v>
+        <v>75</v>
       </c>
       <c r="D12">
         <v>396</v>
       </c>
       <c r="E12">
-        <v>128.54900000000001</v>
+        <v>128.549</v>
       </c>
       <c r="F12" t="s">
-        <v>42</v>
+        <v>64</v>
       </c>
       <c r="G12" t="s">
-        <v>43</v>
+        <v>65</v>
       </c>
       <c r="H12" t="s">
-        <v>44</v>
-      </c>
-      <c r="J12">
+        <v>66</v>
+      </c>
+      <c r="K12">
         <v>0.3452806057714905</v>
       </c>
+      <c r="L12">
+        <v>202.346</v>
+      </c>
+      <c r="M12">
+        <v>-0.3565999999999975</v>
+      </c>
+      <c r="N12">
+        <v>4</v>
+      </c>
+      <c r="O12">
+        <v>4</v>
+      </c>
+      <c r="P12">
+        <v>76.09999999999999</v>
+      </c>
+      <c r="Q12">
+        <v>11</v>
+      </c>
+      <c r="R12">
+        <v>0</v>
+      </c>
+      <c r="S12">
+        <v>1</v>
+      </c>
+      <c r="T12">
+        <v>0</v>
+      </c>
+      <c r="U12">
+        <v>0</v>
+      </c>
+      <c r="V12">
+        <v>0</v>
+      </c>
+      <c r="W12">
+        <v>0</v>
+      </c>
+      <c r="X12">
+        <v>4</v>
+      </c>
+      <c r="Y12">
+        <v>0</v>
+      </c>
+      <c r="Z12">
+        <v>1</v>
+      </c>
+      <c r="AA12">
+        <v>62.31620000000004</v>
+      </c>
+      <c r="AB12">
+        <v>0.09374911607530625</v>
+      </c>
+      <c r="AC12">
+        <v>0.9485411395451377</v>
+      </c>
+      <c r="AD12" t="s">
+        <v>36</v>
+      </c>
     </row>
-    <row r="13" spans="1:10" ht="150" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:30" ht="150" customHeight="1">
       <c r="A13" t="s">
-        <v>51</v>
+        <v>73</v>
       </c>
       <c r="B13" t="s">
-        <v>52</v>
+        <v>74</v>
       </c>
       <c r="C13" t="s">
-        <v>53</v>
+        <v>75</v>
       </c>
       <c r="D13">
         <v>396</v>
       </c>
       <c r="E13">
-        <v>128.54900000000001</v>
+        <v>128.549</v>
       </c>
       <c r="F13" t="s">
+        <v>58</v>
+      </c>
+      <c r="G13" t="s">
+        <v>59</v>
+      </c>
+      <c r="H13" t="s">
+        <v>60</v>
+      </c>
+      <c r="K13">
+        <v>0.5664580841045198</v>
+      </c>
+      <c r="L13">
+        <v>238.309</v>
+      </c>
+      <c r="M13">
+        <v>-1.515899999999997</v>
+      </c>
+      <c r="N13">
+        <v>6</v>
+      </c>
+      <c r="O13">
+        <v>2</v>
+      </c>
+      <c r="P13">
+        <v>81.08</v>
+      </c>
+      <c r="Q13">
+        <v>5</v>
+      </c>
+      <c r="R13">
+        <v>0</v>
+      </c>
+      <c r="S13">
+        <v>1</v>
+      </c>
+      <c r="T13">
+        <v>1</v>
+      </c>
+      <c r="U13">
+        <v>0</v>
+      </c>
+      <c r="V13">
+        <v>0</v>
+      </c>
+      <c r="W13">
+        <v>1</v>
+      </c>
+      <c r="X13">
+        <v>7</v>
+      </c>
+      <c r="Y13">
+        <v>0</v>
+      </c>
+      <c r="Z13">
+        <v>1</v>
+      </c>
+      <c r="AA13">
+        <v>56.38140000000003</v>
+      </c>
+      <c r="AB13">
+        <v>0.1038583819352762</v>
+      </c>
+      <c r="AC13">
+        <v>0.9875519247059777</v>
+      </c>
+      <c r="AD13" t="s">
         <v>36</v>
       </c>
-      <c r="G13" t="s">
-        <v>37</v>
-      </c>
-      <c r="H13" t="s">
-        <v>38</v>
-      </c>
-      <c r="J13">
-        <v>0.56645808410451981</v>
-      </c>
     </row>
-    <row r="14" spans="1:10" ht="150" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:30" ht="150" customHeight="1">
       <c r="A14" t="s">
-        <v>54</v>
+        <v>76</v>
       </c>
       <c r="B14" t="s">
-        <v>55</v>
+        <v>77</v>
       </c>
       <c r="C14" t="s">
-        <v>56</v>
+        <v>78</v>
       </c>
       <c r="D14">
         <v>394</v>
@@ -1809,27 +3208,84 @@
         <v>127.992</v>
       </c>
       <c r="F14" t="s">
-        <v>42</v>
+        <v>64</v>
       </c>
       <c r="G14" t="s">
-        <v>43</v>
+        <v>65</v>
       </c>
       <c r="H14" t="s">
-        <v>44</v>
-      </c>
-      <c r="J14">
+        <v>66</v>
+      </c>
+      <c r="K14">
         <v>0.3452806057714905</v>
       </c>
+      <c r="L14">
+        <v>202.346</v>
+      </c>
+      <c r="M14">
+        <v>-0.3565999999999975</v>
+      </c>
+      <c r="N14">
+        <v>4</v>
+      </c>
+      <c r="O14">
+        <v>4</v>
+      </c>
+      <c r="P14">
+        <v>76.09999999999999</v>
+      </c>
+      <c r="Q14">
+        <v>11</v>
+      </c>
+      <c r="R14">
+        <v>0</v>
+      </c>
+      <c r="S14">
+        <v>1</v>
+      </c>
+      <c r="T14">
+        <v>0</v>
+      </c>
+      <c r="U14">
+        <v>0</v>
+      </c>
+      <c r="V14">
+        <v>0</v>
+      </c>
+      <c r="W14">
+        <v>0</v>
+      </c>
+      <c r="X14">
+        <v>4</v>
+      </c>
+      <c r="Y14">
+        <v>0</v>
+      </c>
+      <c r="Z14">
+        <v>1</v>
+      </c>
+      <c r="AA14">
+        <v>62.31620000000004</v>
+      </c>
+      <c r="AB14">
+        <v>0.07810085167447188</v>
+      </c>
+      <c r="AC14">
+        <v>0.9765957403923328</v>
+      </c>
+      <c r="AD14" t="s">
+        <v>36</v>
+      </c>
     </row>
-    <row r="15" spans="1:10" ht="150" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:30" ht="150" customHeight="1">
       <c r="A15" t="s">
-        <v>54</v>
+        <v>76</v>
       </c>
       <c r="B15" t="s">
-        <v>55</v>
+        <v>77</v>
       </c>
       <c r="C15" t="s">
-        <v>56</v>
+        <v>78</v>
       </c>
       <c r="D15">
         <v>394</v>
@@ -1838,27 +3294,84 @@
         <v>127.992</v>
       </c>
       <c r="F15" t="s">
+        <v>58</v>
+      </c>
+      <c r="G15" t="s">
+        <v>59</v>
+      </c>
+      <c r="H15" t="s">
+        <v>60</v>
+      </c>
+      <c r="K15">
+        <v>0.5664580841045198</v>
+      </c>
+      <c r="L15">
+        <v>238.309</v>
+      </c>
+      <c r="M15">
+        <v>-1.515899999999997</v>
+      </c>
+      <c r="N15">
+        <v>6</v>
+      </c>
+      <c r="O15">
+        <v>2</v>
+      </c>
+      <c r="P15">
+        <v>81.08</v>
+      </c>
+      <c r="Q15">
+        <v>5</v>
+      </c>
+      <c r="R15">
+        <v>0</v>
+      </c>
+      <c r="S15">
+        <v>1</v>
+      </c>
+      <c r="T15">
+        <v>1</v>
+      </c>
+      <c r="U15">
+        <v>0</v>
+      </c>
+      <c r="V15">
+        <v>0</v>
+      </c>
+      <c r="W15">
+        <v>1</v>
+      </c>
+      <c r="X15">
+        <v>7</v>
+      </c>
+      <c r="Y15">
+        <v>0</v>
+      </c>
+      <c r="Z15">
+        <v>1</v>
+      </c>
+      <c r="AA15">
+        <v>56.38140000000003</v>
+      </c>
+      <c r="AB15">
+        <v>0.1143921166112965</v>
+      </c>
+      <c r="AC15">
+        <v>0.9817820684052853</v>
+      </c>
+      <c r="AD15" t="s">
         <v>36</v>
       </c>
-      <c r="G15" t="s">
-        <v>37</v>
-      </c>
-      <c r="H15" t="s">
-        <v>38</v>
-      </c>
-      <c r="J15">
-        <v>0.56645808410451981</v>
-      </c>
     </row>
-    <row r="16" spans="1:10" ht="150" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:30" ht="150" customHeight="1">
       <c r="A16" t="s">
-        <v>57</v>
+        <v>79</v>
       </c>
       <c r="B16" t="s">
-        <v>58</v>
+        <v>80</v>
       </c>
       <c r="C16" t="s">
-        <v>59</v>
+        <v>81</v>
       </c>
       <c r="D16">
         <v>394</v>
@@ -1867,27 +3380,84 @@
         <v>127.992</v>
       </c>
       <c r="F16" t="s">
+        <v>58</v>
+      </c>
+      <c r="G16" t="s">
+        <v>59</v>
+      </c>
+      <c r="H16" t="s">
+        <v>60</v>
+      </c>
+      <c r="K16">
+        <v>0.5664580841045198</v>
+      </c>
+      <c r="L16">
+        <v>238.309</v>
+      </c>
+      <c r="M16">
+        <v>-1.515899999999997</v>
+      </c>
+      <c r="N16">
+        <v>6</v>
+      </c>
+      <c r="O16">
+        <v>2</v>
+      </c>
+      <c r="P16">
+        <v>81.08</v>
+      </c>
+      <c r="Q16">
+        <v>5</v>
+      </c>
+      <c r="R16">
+        <v>0</v>
+      </c>
+      <c r="S16">
+        <v>1</v>
+      </c>
+      <c r="T16">
+        <v>1</v>
+      </c>
+      <c r="U16">
+        <v>0</v>
+      </c>
+      <c r="V16">
+        <v>0</v>
+      </c>
+      <c r="W16">
+        <v>1</v>
+      </c>
+      <c r="X16">
+        <v>7</v>
+      </c>
+      <c r="Y16">
+        <v>0</v>
+      </c>
+      <c r="Z16">
+        <v>1</v>
+      </c>
+      <c r="AA16">
+        <v>56.38140000000003</v>
+      </c>
+      <c r="AB16">
+        <v>0.08606037216313518</v>
+      </c>
+      <c r="AC16">
+        <v>0.9829768018848115</v>
+      </c>
+      <c r="AD16" t="s">
         <v>36</v>
       </c>
-      <c r="G16" t="s">
-        <v>37</v>
-      </c>
-      <c r="H16" t="s">
-        <v>38</v>
-      </c>
-      <c r="J16">
-        <v>0.56645808410451981</v>
-      </c>
     </row>
-    <row r="17" spans="1:10" ht="150" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:30" ht="150" customHeight="1">
       <c r="A17" t="s">
-        <v>60</v>
+        <v>82</v>
       </c>
       <c r="B17" t="s">
-        <v>61</v>
+        <v>83</v>
       </c>
       <c r="C17" t="s">
-        <v>62</v>
+        <v>84</v>
       </c>
       <c r="D17">
         <v>393</v>
@@ -1896,27 +3466,84 @@
         <v>127.687</v>
       </c>
       <c r="F17" t="s">
+        <v>58</v>
+      </c>
+      <c r="G17" t="s">
+        <v>59</v>
+      </c>
+      <c r="H17" t="s">
+        <v>60</v>
+      </c>
+      <c r="K17">
+        <v>0.5664580841045198</v>
+      </c>
+      <c r="L17">
+        <v>238.309</v>
+      </c>
+      <c r="M17">
+        <v>-1.515899999999997</v>
+      </c>
+      <c r="N17">
+        <v>6</v>
+      </c>
+      <c r="O17">
+        <v>2</v>
+      </c>
+      <c r="P17">
+        <v>81.08</v>
+      </c>
+      <c r="Q17">
+        <v>5</v>
+      </c>
+      <c r="R17">
+        <v>0</v>
+      </c>
+      <c r="S17">
+        <v>1</v>
+      </c>
+      <c r="T17">
+        <v>1</v>
+      </c>
+      <c r="U17">
+        <v>0</v>
+      </c>
+      <c r="V17">
+        <v>0</v>
+      </c>
+      <c r="W17">
+        <v>1</v>
+      </c>
+      <c r="X17">
+        <v>7</v>
+      </c>
+      <c r="Y17">
+        <v>0</v>
+      </c>
+      <c r="Z17">
+        <v>1</v>
+      </c>
+      <c r="AA17">
+        <v>56.38140000000003</v>
+      </c>
+      <c r="AB17">
+        <v>0.2963071560976631</v>
+      </c>
+      <c r="AC17">
+        <v>0.8647027657329102</v>
+      </c>
+      <c r="AD17" t="s">
         <v>36</v>
       </c>
-      <c r="G17" t="s">
-        <v>37</v>
-      </c>
-      <c r="H17" t="s">
-        <v>38</v>
-      </c>
-      <c r="J17">
-        <v>0.56645808410451981</v>
-      </c>
     </row>
-    <row r="18" spans="1:10" ht="150" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:30" ht="150" customHeight="1">
       <c r="A18" t="s">
-        <v>60</v>
+        <v>82</v>
       </c>
       <c r="B18" t="s">
-        <v>61</v>
+        <v>83</v>
       </c>
       <c r="C18" t="s">
-        <v>62</v>
+        <v>84</v>
       </c>
       <c r="D18">
         <v>393</v>
@@ -1925,74 +3552,245 @@
         <v>127.687</v>
       </c>
       <c r="F18" t="s">
-        <v>42</v>
+        <v>64</v>
       </c>
       <c r="G18" t="s">
-        <v>43</v>
+        <v>65</v>
       </c>
       <c r="H18" t="s">
-        <v>44</v>
-      </c>
-      <c r="J18">
+        <v>66</v>
+      </c>
+      <c r="K18">
         <v>0.3452806057714905</v>
       </c>
+      <c r="L18">
+        <v>202.346</v>
+      </c>
+      <c r="M18">
+        <v>-0.3565999999999975</v>
+      </c>
+      <c r="N18">
+        <v>4</v>
+      </c>
+      <c r="O18">
+        <v>4</v>
+      </c>
+      <c r="P18">
+        <v>76.09999999999999</v>
+      </c>
+      <c r="Q18">
+        <v>11</v>
+      </c>
+      <c r="R18">
+        <v>0</v>
+      </c>
+      <c r="S18">
+        <v>1</v>
+      </c>
+      <c r="T18">
+        <v>0</v>
+      </c>
+      <c r="U18">
+        <v>0</v>
+      </c>
+      <c r="V18">
+        <v>0</v>
+      </c>
+      <c r="W18">
+        <v>0</v>
+      </c>
+      <c r="X18">
+        <v>4</v>
+      </c>
+      <c r="Y18">
+        <v>0</v>
+      </c>
+      <c r="Z18">
+        <v>1</v>
+      </c>
+      <c r="AA18">
+        <v>62.31620000000004</v>
+      </c>
+      <c r="AB18">
+        <v>0.1333072251329742</v>
+      </c>
+      <c r="AC18">
+        <v>0.9284643410077315</v>
+      </c>
+      <c r="AD18" t="s">
+        <v>36</v>
+      </c>
     </row>
-    <row r="19" spans="1:10" ht="150" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:30" ht="150" customHeight="1">
       <c r="A19" t="s">
-        <v>63</v>
+        <v>85</v>
       </c>
       <c r="B19" t="s">
-        <v>64</v>
+        <v>86</v>
       </c>
       <c r="C19" t="s">
-        <v>65</v>
+        <v>87</v>
       </c>
       <c r="D19">
         <v>393</v>
       </c>
       <c r="E19">
-        <v>127.64700000000001</v>
+        <v>127.647</v>
       </c>
       <c r="F19" t="s">
-        <v>42</v>
+        <v>64</v>
       </c>
       <c r="G19" t="s">
-        <v>43</v>
+        <v>65</v>
       </c>
       <c r="H19" t="s">
-        <v>44</v>
-      </c>
-      <c r="J19">
+        <v>66</v>
+      </c>
+      <c r="K19">
         <v>0.3452806057714905</v>
       </c>
+      <c r="L19">
+        <v>202.346</v>
+      </c>
+      <c r="M19">
+        <v>-0.3565999999999975</v>
+      </c>
+      <c r="N19">
+        <v>4</v>
+      </c>
+      <c r="O19">
+        <v>4</v>
+      </c>
+      <c r="P19">
+        <v>76.09999999999999</v>
+      </c>
+      <c r="Q19">
+        <v>11</v>
+      </c>
+      <c r="R19">
+        <v>0</v>
+      </c>
+      <c r="S19">
+        <v>1</v>
+      </c>
+      <c r="T19">
+        <v>0</v>
+      </c>
+      <c r="U19">
+        <v>0</v>
+      </c>
+      <c r="V19">
+        <v>0</v>
+      </c>
+      <c r="W19">
+        <v>0</v>
+      </c>
+      <c r="X19">
+        <v>4</v>
+      </c>
+      <c r="Y19">
+        <v>0</v>
+      </c>
+      <c r="Z19">
+        <v>1</v>
+      </c>
+      <c r="AA19">
+        <v>62.31620000000004</v>
+      </c>
+      <c r="AB19">
+        <v>0.1554410343038993</v>
+      </c>
+      <c r="AC19">
+        <v>0.9428078727796092</v>
+      </c>
+      <c r="AD19" t="s">
+        <v>36</v>
+      </c>
     </row>
-    <row r="20" spans="1:10" ht="150" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:30" ht="150" customHeight="1">
       <c r="A20" t="s">
-        <v>63</v>
+        <v>85</v>
       </c>
       <c r="B20" t="s">
-        <v>64</v>
+        <v>86</v>
       </c>
       <c r="C20" t="s">
-        <v>65</v>
+        <v>87</v>
       </c>
       <c r="D20">
         <v>393</v>
       </c>
       <c r="E20">
-        <v>127.64700000000001</v>
+        <v>127.647</v>
       </c>
       <c r="F20" t="s">
+        <v>58</v>
+      </c>
+      <c r="G20" t="s">
+        <v>59</v>
+      </c>
+      <c r="H20" t="s">
+        <v>60</v>
+      </c>
+      <c r="K20">
+        <v>0.5664580841045198</v>
+      </c>
+      <c r="L20">
+        <v>238.309</v>
+      </c>
+      <c r="M20">
+        <v>-1.515899999999997</v>
+      </c>
+      <c r="N20">
+        <v>6</v>
+      </c>
+      <c r="O20">
+        <v>2</v>
+      </c>
+      <c r="P20">
+        <v>81.08</v>
+      </c>
+      <c r="Q20">
+        <v>5</v>
+      </c>
+      <c r="R20">
+        <v>0</v>
+      </c>
+      <c r="S20">
+        <v>1</v>
+      </c>
+      <c r="T20">
+        <v>1</v>
+      </c>
+      <c r="U20">
+        <v>0</v>
+      </c>
+      <c r="V20">
+        <v>0</v>
+      </c>
+      <c r="W20">
+        <v>1</v>
+      </c>
+      <c r="X20">
+        <v>7</v>
+      </c>
+      <c r="Y20">
+        <v>0</v>
+      </c>
+      <c r="Z20">
+        <v>1</v>
+      </c>
+      <c r="AA20">
+        <v>56.38140000000003</v>
+      </c>
+      <c r="AB20">
+        <v>0.1195498370459797</v>
+      </c>
+      <c r="AC20">
+        <v>0.9947176706272823</v>
+      </c>
+      <c r="AD20" t="s">
         <v>36</v>
-      </c>
-      <c r="G20" t="s">
-        <v>37</v>
-      </c>
-      <c r="H20" t="s">
-        <v>38</v>
-      </c>
-      <c r="J20">
-        <v>0.56645808410451981</v>
       </c>
     </row>
   </sheetData>

</xml_diff>